<commit_message>
add more data in the file
</commit_message>
<xml_diff>
--- a/data/chepai.xlsx
+++ b/data/chepai.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="91">
   <si>
     <t>2014年1月</t>
   </si>
@@ -140,72 +140,39 @@
     <t>%2013_1</t>
   </si>
   <si>
-    <t>11：29：40</t>
-  </si>
-  <si>
     <t>%2013_2</t>
   </si>
   <si>
-    <t>11：29：59</t>
-  </si>
-  <si>
     <t>%2013_3</t>
   </si>
   <si>
-    <t>11：29：44</t>
-  </si>
-  <si>
     <t>2013_4</t>
   </si>
   <si>
-    <t>11：27：04</t>
-  </si>
-  <si>
     <t>2013_5</t>
   </si>
   <si>
-    <t>11：29：26</t>
-  </si>
-  <si>
     <t>2013_6</t>
   </si>
   <si>
-    <t>11：21：22</t>
-  </si>
-  <si>
     <t>2013_7</t>
   </si>
   <si>
-    <t>11：29：22</t>
-  </si>
-  <si>
     <t>2013_8</t>
   </si>
   <si>
-    <t>11：29：24</t>
-  </si>
-  <si>
     <t>2013_9</t>
   </si>
   <si>
     <t>%2013_10</t>
   </si>
   <si>
-    <t>11：29：56</t>
-  </si>
-  <si>
     <t>2013_11</t>
   </si>
   <si>
-    <t>11：29：34</t>
-  </si>
-  <si>
     <t>2013_12</t>
   </si>
   <si>
-    <t>11：29：50</t>
-  </si>
-  <si>
     <t>2014_1</t>
   </si>
   <si>
@@ -252,6 +219,75 @@
   </si>
   <si>
     <t>2015_4</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>投标人数/投放数量</t>
+  </si>
+  <si>
+    <t>最低成交价-警示价格</t>
+  </si>
+  <si>
+    <t>平均成交价-警示价格</t>
+  </si>
+  <si>
+    <t>29.40</t>
+  </si>
+  <si>
+    <t>29.59</t>
+  </si>
+  <si>
+    <t>29.44</t>
+  </si>
+  <si>
+    <t>29.26</t>
+  </si>
+  <si>
+    <t>29.22</t>
+  </si>
+  <si>
+    <t>29.24</t>
+  </si>
+  <si>
+    <t>29.56</t>
+  </si>
+  <si>
+    <t>29.34</t>
+  </si>
+  <si>
+    <t>29.50</t>
+  </si>
+  <si>
+    <t>27.04</t>
+  </si>
+  <si>
+    <t>21.22</t>
+  </si>
+  <si>
+    <t>29.54</t>
+  </si>
+  <si>
+    <t>29.48</t>
+  </si>
+  <si>
+    <t>29.45</t>
+  </si>
+  <si>
+    <t>29.52</t>
+  </si>
+  <si>
+    <t>29.49</t>
+  </si>
+  <si>
+    <t>29.41</t>
+  </si>
+  <si>
+    <t>20.16</t>
+  </si>
+  <si>
+    <t>02.48</t>
   </si>
 </sst>
 </file>
@@ -267,12 +303,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -287,9 +335,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,52 +882,52 @@
                 <c:formatCode>h:mm:ss</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.47915509259259265</c:v>
+                  <c:v>29.59</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.47898148148148145</c:v>
+                  <c:v>29.44</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47902777777777777</c:v>
+                  <c:v>29.48</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.47899305555555555</c:v>
+                  <c:v>29.45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.47902777777777777</c:v>
+                  <c:v>29.48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.47899305555555555</c:v>
+                  <c:v>29.45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.47915509259259265</c:v>
+                  <c:v>29.59</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.47898148148148145</c:v>
+                  <c:v>29.44</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.47907407407407404</c:v>
+                  <c:v>29.52</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.47915509259259265</c:v>
+                  <c:v>29.59</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.47905092592592591</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.47912037037037036</c:v>
+                  <c:v>29.56</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.46027777777777779</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.47903935185185187</c:v>
+                  <c:v>29.49</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.47240740740740739</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.47894675925925928</c:v>
+                  <c:v>29.41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1279,11 +1335,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="199327072"/>
-        <c:axId val="199300696"/>
+        <c:axId val="203768152"/>
+        <c:axId val="204334400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199327072"/>
+        <c:axId val="203768152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1326,7 +1382,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199300696"/>
+        <c:crossAx val="204334400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1334,7 +1390,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199300696"/>
+        <c:axId val="204334400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1385,7 +1441,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199327072"/>
+        <c:crossAx val="203768152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2344,13 +2400,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2392,7 +2455,7 @@
         <v>73501</v>
       </c>
       <c r="E2" s="1">
-        <v>0.47915509259259265</v>
+        <v>29.59</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
@@ -2418,7 +2481,7 @@
         <v>73357</v>
       </c>
       <c r="E3" s="1">
-        <v>0.47898148148148145</v>
+        <v>29.44</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
@@ -2444,7 +2507,7 @@
         <v>73872</v>
       </c>
       <c r="E4" s="1">
-        <v>0.47902777777777777</v>
+        <v>29.48</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
@@ -2470,7 +2533,7 @@
         <v>74113</v>
       </c>
       <c r="E5" s="1">
-        <v>0.47899305555555555</v>
+        <v>29.45</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -2496,7 +2559,7 @@
         <v>74503</v>
       </c>
       <c r="E6" s="1">
-        <v>0.47902777777777777</v>
+        <v>29.48</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -2522,7 +2585,7 @@
         <v>73896</v>
       </c>
       <c r="E7" s="1">
-        <v>0.47899305555555555</v>
+        <v>29.45</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -2548,7 +2611,7 @@
         <v>74680</v>
       </c>
       <c r="E8" s="1">
-        <v>0.47915509259259265</v>
+        <v>29.59</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -2574,7 +2637,7 @@
         <v>73785</v>
       </c>
       <c r="E9" s="1">
-        <v>0.47898148148148145</v>
+        <v>29.44</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
@@ -2600,7 +2663,7 @@
         <v>73875</v>
       </c>
       <c r="E10" s="1">
-        <v>0.47907407407407404</v>
+        <v>29.52</v>
       </c>
       <c r="F10" t="s">
         <v>17</v>
@@ -2626,7 +2689,7 @@
         <v>74075</v>
       </c>
       <c r="E11" s="1">
-        <v>0.47915509259259265</v>
+        <v>29.59</v>
       </c>
       <c r="F11" t="s">
         <v>19</v>
@@ -2652,7 +2715,7 @@
         <v>73633</v>
       </c>
       <c r="E12" s="1">
-        <v>0.47905092592592591</v>
+        <v>29.5</v>
       </c>
       <c r="F12" t="s">
         <v>21</v>
@@ -2678,7 +2741,7 @@
         <v>73687</v>
       </c>
       <c r="E13" s="1">
-        <v>0.47912037037037036</v>
+        <v>29.56</v>
       </c>
       <c r="F13" t="s">
         <v>23</v>
@@ -2730,7 +2793,7 @@
         <v>76618</v>
       </c>
       <c r="E15" s="1">
-        <v>0.47903935185185187</v>
+        <v>29.49</v>
       </c>
       <c r="F15" t="s">
         <v>27</v>
@@ -2768,7 +2831,7 @@
         <v>73700</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2782,7 +2845,7 @@
         <v>80759</v>
       </c>
       <c r="E17" s="1">
-        <v>0.47894675925925928</v>
+        <v>29.41</v>
       </c>
       <c r="F17" t="s">
         <v>31</v>
@@ -2794,99 +2857,158 @@
         <v>75200</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" t="s">
+        <v>37</v>
+      </c>
+      <c r="G31" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="4">
         <v>9000</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="4">
         <v>75000</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="4">
         <v>75332</v>
       </c>
-      <c r="F32" t="s">
-        <v>41</v>
-      </c>
-      <c r="G32">
+      <c r="F32" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" s="4">
         <v>65</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="4">
         <v>20857</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="4">
         <v>0</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="4">
         <f>H32/C32</f>
         <v>2.3174444444444444</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33">
+      <c r="K32" s="4">
+        <f>D32-I32</f>
+        <v>75000</v>
+      </c>
+      <c r="L32" s="4">
+        <f>E32-I32</f>
+        <v>75332</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="4">
         <v>9000</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="4">
         <v>83300</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="4">
         <v>83571</v>
       </c>
-      <c r="F33" t="s">
-        <v>43</v>
-      </c>
-      <c r="G33">
+      <c r="F33" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" s="4">
         <v>113</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="4">
         <v>24651</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="4">
         <v>0</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="4">
         <f t="shared" ref="J33:J59" si="0">H33/C33</f>
         <v>2.7389999999999999</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34">
+      <c r="K33" s="4">
+        <f t="shared" ref="K33:K59" si="1">D33-I33</f>
+        <v>83300</v>
+      </c>
+      <c r="L33" s="4">
+        <f t="shared" ref="L33:L59" si="2">E33-I33</f>
+        <v>83571</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="4">
         <v>9000</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="4">
         <v>90800</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="4">
         <v>91898</v>
       </c>
-      <c r="F34" t="s">
-        <v>45</v>
-      </c>
-      <c r="G34">
+      <c r="F34" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G34" s="4">
         <v>1</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="4">
         <v>23589</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="4">
         <v>0</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="4">
         <f t="shared" si="0"/>
         <v>2.621</v>
       </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="4">
+        <f t="shared" si="1"/>
+        <v>90800</v>
+      </c>
+      <c r="L34" s="4">
+        <f t="shared" si="2"/>
+        <v>91898</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C35">
         <v>11000</v>
@@ -2897,8 +3019,8 @@
       <c r="E35">
         <v>84101</v>
       </c>
-      <c r="F35" t="s">
-        <v>47</v>
+      <c r="F35" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="G35">
         <v>3</v>
@@ -2913,10 +3035,18 @@
         <f t="shared" si="0"/>
         <v>2.3794545454545455</v>
       </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="L35" s="4">
+        <f t="shared" si="2"/>
+        <v>501</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C36">
         <v>9000</v>
@@ -2927,8 +3057,8 @@
       <c r="E36">
         <v>80803</v>
       </c>
-      <c r="F36" t="s">
-        <v>49</v>
+      <c r="F36" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="G36">
         <v>4</v>
@@ -2943,10 +3073,18 @@
         <f t="shared" si="0"/>
         <v>2.4693333333333332</v>
       </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K36">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+      <c r="L36" s="4">
+        <f t="shared" si="2"/>
+        <v>903</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C37">
         <v>9000</v>
@@ -2957,8 +3095,8 @@
       <c r="E37">
         <v>77823</v>
       </c>
-      <c r="F37" t="s">
-        <v>51</v>
+      <c r="F37" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -2973,10 +3111,18 @@
         <f t="shared" si="0"/>
         <v>2.3868888888888891</v>
       </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K37">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="L37" s="4">
+        <f t="shared" si="2"/>
+        <v>523</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C38">
         <v>9000</v>
@@ -2987,8 +3133,8 @@
       <c r="E38">
         <v>76465</v>
       </c>
-      <c r="F38" t="s">
-        <v>53</v>
+      <c r="F38" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="G38">
         <v>933</v>
@@ -3003,10 +3149,18 @@
         <f t="shared" si="0"/>
         <v>2.4234444444444443</v>
       </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+      <c r="L38" s="4">
+        <f t="shared" si="2"/>
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C39">
         <v>9000</v>
@@ -3017,8 +3171,8 @@
       <c r="E39">
         <v>74939</v>
       </c>
-      <c r="F39" t="s">
-        <v>55</v>
+      <c r="F39" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="G39">
         <v>30</v>
@@ -3033,10 +3187,18 @@
         <f t="shared" si="0"/>
         <v>2.5166666666666666</v>
       </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K39">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="L39" s="4">
+        <f t="shared" si="2"/>
+        <v>839</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C40">
         <v>9000</v>
@@ -3047,8 +3209,8 @@
       <c r="E40">
         <v>73492</v>
       </c>
-      <c r="F40" s="1">
-        <v>0.47909722222222223</v>
+      <c r="F40" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="G40">
         <v>96</v>
@@ -3063,40 +3225,56 @@
         <f t="shared" si="0"/>
         <v>3.9060000000000001</v>
       </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41">
+      <c r="K40">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+      <c r="L40" s="4">
+        <f t="shared" si="2"/>
+        <v>892</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="4">
         <v>10000</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="4">
         <v>82300</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="4">
         <v>83723</v>
       </c>
-      <c r="F41" t="s">
-        <v>58</v>
-      </c>
-      <c r="G41">
+      <c r="F41" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G41" s="4">
         <v>309</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="4">
         <v>28887</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="4">
         <v>0</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="4">
         <f t="shared" si="0"/>
         <v>2.8887</v>
       </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K41" s="4">
+        <f t="shared" si="1"/>
+        <v>82300</v>
+      </c>
+      <c r="L41" s="4">
+        <f t="shared" si="2"/>
+        <v>83723</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C42">
         <v>8500</v>
@@ -3107,8 +3285,8 @@
       <c r="E42">
         <v>75717</v>
       </c>
-      <c r="F42" t="s">
-        <v>60</v>
+      <c r="F42" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="G42">
         <v>5</v>
@@ -3123,10 +3301,18 @@
         <f t="shared" si="0"/>
         <v>4.4964705882352938</v>
       </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K42">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="L42" s="4">
+        <f t="shared" si="2"/>
+        <v>817</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C43">
         <v>8500</v>
@@ -3137,8 +3323,8 @@
       <c r="E43">
         <v>76093</v>
       </c>
-      <c r="F43" t="s">
-        <v>62</v>
+      <c r="F43" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="G43">
         <v>13</v>
@@ -3153,10 +3339,18 @@
         <f t="shared" si="0"/>
         <v>4.6617647058823533</v>
       </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K43">
+        <f t="shared" si="1"/>
+        <v>1100</v>
+      </c>
+      <c r="L43" s="4">
+        <f t="shared" si="2"/>
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C44">
         <v>8100</v>
@@ -3167,8 +3361,8 @@
       <c r="E44">
         <v>73501</v>
       </c>
-      <c r="F44" s="1">
-        <v>0.47915509259259265</v>
+      <c r="F44" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="G44">
         <v>158</v>
@@ -3183,10 +3377,18 @@
         <f t="shared" si="0"/>
         <v>5.1785185185185183</v>
       </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K44">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+      <c r="L44" s="4">
+        <f t="shared" si="2"/>
+        <v>901</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C45">
         <v>7400</v>
@@ -3197,8 +3399,8 @@
       <c r="E45">
         <v>73357</v>
       </c>
-      <c r="F45" s="1">
-        <v>0.47898148148148145</v>
+      <c r="F45" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="G45">
         <v>347</v>
@@ -3213,10 +3415,18 @@
         <f t="shared" si="0"/>
         <v>6.1835135135135131</v>
       </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K45">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="L45" s="4">
+        <f t="shared" si="2"/>
+        <v>757</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C46">
         <v>7400</v>
@@ -3227,8 +3437,8 @@
       <c r="E46">
         <v>73872</v>
       </c>
-      <c r="F46" s="1">
-        <v>0.47902777777777777</v>
+      <c r="F46" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="G46">
         <v>259</v>
@@ -3243,10 +3453,18 @@
         <f t="shared" si="0"/>
         <v>8.3585135135135129</v>
       </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K46">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+      <c r="L46" s="4">
+        <f t="shared" si="2"/>
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C47">
         <v>8200</v>
@@ -3257,8 +3475,8 @@
       <c r="E47">
         <v>74113</v>
       </c>
-      <c r="F47" s="1">
-        <v>0.47899305555555555</v>
+      <c r="F47" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="G47">
         <v>44</v>
@@ -3273,10 +3491,18 @@
         <f t="shared" si="0"/>
         <v>11.49280487804878</v>
       </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K47">
+        <f t="shared" si="1"/>
+        <v>1400</v>
+      </c>
+      <c r="L47" s="4">
+        <f t="shared" si="2"/>
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C48">
         <v>7400</v>
@@ -3287,8 +3513,8 @@
       <c r="E48">
         <v>74503</v>
       </c>
-      <c r="F48" s="1">
-        <v>0.47902777777777777</v>
+      <c r="F48" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="G48">
         <v>219</v>
@@ -3303,10 +3529,18 @@
         <f t="shared" si="0"/>
         <v>15.421756756756757</v>
       </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K48">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+      <c r="L48" s="4">
+        <f>E48-I48</f>
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C49">
         <v>7400</v>
@@ -3317,8 +3551,8 @@
       <c r="E49">
         <v>73896</v>
       </c>
-      <c r="F49" s="1">
-        <v>0.47899305555555555</v>
+      <c r="F49" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="G49">
         <v>238</v>
@@ -3333,10 +3567,18 @@
         <f t="shared" si="0"/>
         <v>18.33472972972973</v>
       </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K49">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+      <c r="L49" s="4">
+        <f t="shared" si="2"/>
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C50">
         <v>7400</v>
@@ -3347,8 +3589,8 @@
       <c r="E50">
         <v>74680</v>
       </c>
-      <c r="F50" s="1">
-        <v>0.47915509259259265</v>
+      <c r="F50" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="G50">
         <v>23</v>
@@ -3363,10 +3605,18 @@
         <f t="shared" si="0"/>
         <v>18.391621621621621</v>
       </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K50">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="L50" s="4">
+        <f t="shared" si="2"/>
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C51">
         <v>7400</v>
@@ -3377,8 +3627,8 @@
       <c r="E51">
         <v>73785</v>
       </c>
-      <c r="F51" s="1">
-        <v>0.47898148148148145</v>
+      <c r="F51" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="G51">
         <v>53</v>
@@ -3393,10 +3643,18 @@
         <f t="shared" si="0"/>
         <v>16.425675675675677</v>
       </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K51">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="L51" s="4">
+        <f t="shared" si="2"/>
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C52">
         <v>8300</v>
@@ -3407,8 +3665,8 @@
       <c r="E52">
         <v>73875</v>
       </c>
-      <c r="F52" s="1">
-        <v>0.47907407407407404</v>
+      <c r="F52" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="G52">
         <v>183</v>
@@ -3423,10 +3681,18 @@
         <f t="shared" si="0"/>
         <v>14.725180722891567</v>
       </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K52">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+      <c r="L52" s="4">
+        <f t="shared" si="2"/>
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C53">
         <v>7400</v>
@@ -3437,8 +3703,8 @@
       <c r="E53">
         <v>74075</v>
       </c>
-      <c r="F53" s="1">
-        <v>0.47915509259259265</v>
+      <c r="F53" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="G53">
         <v>30</v>
@@ -3453,10 +3719,18 @@
         <f t="shared" si="0"/>
         <v>14.26108108108108</v>
       </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K53">
+        <f t="shared" si="1"/>
+        <v>1400</v>
+      </c>
+      <c r="L53" s="4">
+        <f t="shared" si="2"/>
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C54">
         <v>7400</v>
@@ -3467,8 +3741,8 @@
       <c r="E54">
         <v>73633</v>
       </c>
-      <c r="F54" s="1">
-        <v>0.47905092592592591</v>
+      <c r="F54" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="G54">
         <v>77</v>
@@ -3483,10 +3757,18 @@
         <f t="shared" si="0"/>
         <v>12.918243243243243</v>
       </c>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K54">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+      <c r="L54" s="4">
+        <f t="shared" si="2"/>
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C55">
         <v>7447</v>
@@ -3497,8 +3779,8 @@
       <c r="E55">
         <v>73687</v>
       </c>
-      <c r="F55" s="1">
-        <v>0.47912037037037036</v>
+      <c r="F55" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="G55">
         <v>628</v>
@@ -3513,40 +3795,56 @@
         <f t="shared" si="0"/>
         <v>13.021619444071439</v>
       </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>75</v>
-      </c>
-      <c r="C56">
+      <c r="K55">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="L55" s="4">
+        <f t="shared" si="2"/>
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" s="4">
         <v>7990</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="4">
         <v>74000</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="4">
         <v>74216</v>
       </c>
-      <c r="F56" s="1">
-        <v>0.46027777777777779</v>
-      </c>
-      <c r="G56">
+      <c r="F56" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G56" s="4">
         <v>2</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="4">
         <v>98203</v>
       </c>
-      <c r="I56">
+      <c r="I56" s="4">
         <v>73700</v>
       </c>
-      <c r="J56">
+      <c r="J56" s="4">
         <f t="shared" si="0"/>
         <v>12.290738423028786</v>
       </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K56" s="4">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="L56" s="4">
+        <f t="shared" si="2"/>
+        <v>516</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C57">
         <v>7653</v>
@@ -3557,8 +3855,8 @@
       <c r="E57">
         <v>76618</v>
       </c>
-      <c r="F57" s="1">
-        <v>0.47903935185185187</v>
+      <c r="F57" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="G57">
         <v>73</v>
@@ -3573,40 +3871,56 @@
         <f t="shared" si="0"/>
         <v>13.488043904351235</v>
       </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>77</v>
-      </c>
-      <c r="C58">
+      <c r="K57">
+        <f t="shared" si="1"/>
+        <v>2800</v>
+      </c>
+      <c r="L57" s="4">
+        <f t="shared" si="2"/>
+        <v>2918</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C58" s="4">
         <v>7406</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="4">
         <v>74600</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="4">
         <v>74830</v>
       </c>
-      <c r="F58" s="1">
-        <v>0.47240740740740739</v>
-      </c>
-      <c r="G58">
+      <c r="F58" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G58" s="4">
         <v>6</v>
       </c>
-      <c r="H58">
+      <c r="H58" s="4">
         <v>132690</v>
       </c>
-      <c r="I58">
+      <c r="I58" s="4">
         <v>73700</v>
       </c>
-      <c r="J58">
+      <c r="J58" s="4">
         <f t="shared" si="0"/>
         <v>17.916554145287606</v>
       </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K58" s="4">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+      <c r="L58" s="4">
+        <f t="shared" si="2"/>
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C59">
         <v>8288</v>
@@ -3617,8 +3931,8 @@
       <c r="E59">
         <v>80759</v>
       </c>
-      <c r="F59" s="1">
-        <v>0.47894675925925928</v>
+      <c r="F59" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="G59">
         <v>115</v>
@@ -3633,10 +3947,28 @@
         <f t="shared" si="0"/>
         <v>18.375723938223938</v>
       </c>
+      <c r="K59">
+        <f t="shared" si="1"/>
+        <v>5400</v>
+      </c>
+      <c r="L59" s="4">
+        <f t="shared" si="2"/>
+        <v>5559</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G62" s="9"/>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G63" s="9"/>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G64" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>